<commit_message>
Updating parameters and hard setting sexualkities
</commit_message>
<xml_diff>
--- a/data/excelsheets/Receptive sharing risk.xlsx
+++ b/data/excelsheets/Receptive sharing risk.xlsx
@@ -96,10 +96,10 @@
     <t>Of people who share, number  of times expected to do so</t>
   </si>
   <si>
-    <t xml:space="preserve">Decrease by reaching age 40 </t>
-  </si>
-  <si>
     <t>The relationship between age and risky injecting behaviours among a sample of Australian people who inject drugs.</t>
+  </si>
+  <si>
+    <t>Risk ratio of receptive injection</t>
   </si>
 </sst>
 </file>
@@ -737,11 +737,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169684352"/>
-        <c:axId val="169682816"/>
+        <c:axId val="186244096"/>
+        <c:axId val="174998272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169684352"/>
+        <c:axId val="186244096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,12 +751,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169682816"/>
+        <c:crossAx val="174998272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169682816"/>
+        <c:axId val="174998272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169684352"/>
+        <c:crossAx val="186244096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1115,11 +1115,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174080384"/>
-        <c:axId val="174081920"/>
+        <c:axId val="186198656"/>
+        <c:axId val="186204544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174080384"/>
+        <c:axId val="186198656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174081920"/>
+        <c:crossAx val="186204544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1136,7 +1136,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174081920"/>
+        <c:axId val="186204544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174080384"/>
+        <c:crossAx val="186198656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1524,7 +1524,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2172,79 +2172,79 @@
         <v>19</v>
       </c>
       <c r="B24">
-        <f>SUM(B18:B21)/SUM(B17:B21)</f>
+        <f t="shared" ref="B24:T24" si="3">SUM(B18:B21)/SUM(B17:B21)</f>
         <v>0.31199186991869921</v>
       </c>
       <c r="C24" s="1">
-        <f>SUM(C18:C21)/SUM(C17:C21)</f>
+        <f t="shared" si="3"/>
         <v>0.27463768115942028</v>
       </c>
       <c r="D24" s="1">
-        <f>SUM(D18:D21)/SUM(D17:D21)</f>
+        <f t="shared" si="3"/>
         <v>0.14899713467048711</v>
       </c>
       <c r="E24" s="1">
-        <f>SUM(E18:E21)/SUM(E17:E21)</f>
+        <f t="shared" si="3"/>
         <v>0.17858602370249285</v>
       </c>
       <c r="F24" s="1">
-        <f>SUM(F18:F21)/SUM(F17:F21)</f>
+        <f t="shared" si="3"/>
         <v>0.20275862068965517</v>
       </c>
       <c r="G24" s="1">
-        <f>SUM(G18:G21)/SUM(G17:G21)</f>
+        <f t="shared" si="3"/>
         <v>0.17146433041301626</v>
       </c>
       <c r="H24" s="1">
-        <f>SUM(H18:H21)/SUM(H17:H21)</f>
+        <f t="shared" si="3"/>
         <v>0.15622032288698956</v>
       </c>
       <c r="I24" s="1">
-        <f>SUM(I18:I21)/SUM(I17:I21)</f>
+        <f t="shared" si="3"/>
         <v>0.16295594504973945</v>
       </c>
       <c r="J24" s="1">
-        <f>SUM(J18:J21)/SUM(J17:J21)</f>
+        <f t="shared" si="3"/>
         <v>0.14760147601476015</v>
       </c>
       <c r="K24" s="1">
-        <f>SUM(K18:K21)/SUM(K17:K21)</f>
+        <f t="shared" si="3"/>
         <v>0.18438538205980065</v>
       </c>
       <c r="L24" s="1">
-        <f>SUM(L18:L21)/SUM(L17:L21)</f>
+        <f t="shared" si="3"/>
         <v>0.13449163449163448</v>
       </c>
       <c r="M24" s="1">
-        <f>SUM(M18:M21)/SUM(M17:M21)</f>
+        <f t="shared" si="3"/>
         <v>0.15416420555227406</v>
       </c>
       <c r="N24" s="1">
-        <f>SUM(N18:N21)/SUM(N17:N21)</f>
+        <f t="shared" si="3"/>
         <v>0.15997566909975669</v>
       </c>
       <c r="O24" s="1">
-        <f>SUM(O18:O21)/SUM(O17:O21)</f>
+        <f t="shared" si="3"/>
         <v>0.16919959473150961</v>
       </c>
       <c r="P24" s="1">
-        <f>SUM(P18:P21)/SUM(P17:P21)</f>
+        <f t="shared" si="3"/>
         <v>0.16075245831551946</v>
       </c>
       <c r="Q24" s="1">
-        <f>SUM(Q18:Q21)/SUM(Q17:Q21)</f>
+        <f t="shared" si="3"/>
         <v>0.14108777598276789</v>
       </c>
       <c r="R24" s="1">
-        <f>SUM(R18:R21)/SUM(R17:R21)</f>
+        <f t="shared" si="3"/>
         <v>0.15967660434562911</v>
       </c>
       <c r="S24" s="1">
-        <f>SUM(S18:S21)/SUM(S17:S21)</f>
+        <f t="shared" si="3"/>
         <v>0.16398243045387995</v>
       </c>
       <c r="T24" s="1">
-        <f>SUM(T18:T21)/SUM(T17:T21)</f>
+        <f t="shared" si="3"/>
         <v>0.15067178502879078</v>
       </c>
     </row>
@@ -2278,321 +2278,321 @@
         <v>0.3289902280130293</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:T34" si="3">C18/SUM(C$18:C$21)</f>
+        <f t="shared" ref="C31:T34" si="4">C18/SUM(C$18:C$21)</f>
         <v>0.40897097625329815</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29230769230769232</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34553775743707094</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.37414965986394561</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.37712895377128952</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.37386018237082069</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.32558139534883723</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.37812499999999999</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.33933933933933935</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.28708133971291866</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.33716475095785442</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.39543726235741444</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.32335329341317365</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.32978723404255317</v>
       </c>
       <c r="Q31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.33206106870229007</v>
       </c>
       <c r="R31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.32911392405063289</v>
       </c>
       <c r="S31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44047619047619047</v>
       </c>
       <c r="T31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.33439490445859871</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A32:A34" si="4">A19</f>
+        <f t="shared" ref="A32:A34" si="5">A19</f>
         <v>Twice</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" ref="B32:Q34" si="5">B19/SUM(B$18:B$21)</f>
+        <f t="shared" ref="B32:Q34" si="6">B19/SUM(B$18:B$21)</f>
         <v>0.3289902280130293</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.30606860158311344</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27692307692307694</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.28832951945080093</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.24263038548752835</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27493917274939172</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.23404255319148937</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.29651162790697677</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.22812499999999999</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27627627627627627</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.24521072796934865</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.20152091254752852</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.30239520958083832</v>
       </c>
       <c r="P32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.2473404255319149</v>
       </c>
       <c r="Q32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.26717557251908397</v>
       </c>
       <c r="R32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25316455696202533</v>
       </c>
       <c r="S32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17857142857142858</v>
       </c>
       <c r="T32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25159235668789809</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3-5times</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.23127035830618892</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.16886543535620052</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26923076923076922</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22425629290617849</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.21315192743764172</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.21411192214111921</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.20972644376899696</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.21511627906976744</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.24062500000000001</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.24924924924924924</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26315789473684209</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.23754789272030652</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26615969581749049</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.20958083832335328</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22872340425531915</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22137404580152673</v>
       </c>
       <c r="R33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.23417721518987342</v>
       </c>
       <c r="S33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18154761904761904</v>
       </c>
       <c r="T33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.20063694267515925</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&gt;5times</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.11074918566775244</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.11609498680738786</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.16153846153846155</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.14187643020594964</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17006802721088435</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13381995133819952</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18237082066869301</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.16279069767441862</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15312500000000001</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13513513513513514</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17703349282296652</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18007662835249041</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13688212927756654</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.16467065868263472</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19414893617021275</v>
       </c>
       <c r="Q34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17938931297709923</v>
       </c>
       <c r="R34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18354430379746836</v>
       </c>
       <c r="S34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19940476190476192</v>
       </c>
       <c r="T34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.21337579617834396</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new sharing parameters
</commit_message>
<xml_diff>
--- a/data/excelsheets/Receptive sharing risk.xlsx
+++ b/data/excelsheets/Receptive sharing risk.xlsx
@@ -737,11 +737,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186244096"/>
-        <c:axId val="174998272"/>
+        <c:axId val="43546880"/>
+        <c:axId val="43560960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186244096"/>
+        <c:axId val="43546880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,12 +751,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174998272"/>
+        <c:crossAx val="43560960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174998272"/>
+        <c:axId val="43560960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186244096"/>
+        <c:crossAx val="43546880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1115,11 +1115,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="186198656"/>
-        <c:axId val="186204544"/>
+        <c:axId val="54466432"/>
+        <c:axId val="54467968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="186198656"/>
+        <c:axId val="54466432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186204544"/>
+        <c:crossAx val="54467968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1136,7 +1136,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186204544"/>
+        <c:axId val="54467968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1147,165 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186198656"/>
+        <c:crossAx val="54466432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$T$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.31199186991869921</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27463768115942028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14899713467048711</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17858602370249285</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20275862068965517</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17146433041301626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15622032288698956</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16295594504973945</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14760147601476015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18438538205980065</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13449163449163448</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15416420555227406</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15997566909975669</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16919959473150961</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16075245831551946</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14108777598276789</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15967660434562911</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.16398243045387995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.15067178502879078</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="35055104"/>
+        <c:axId val="35056640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="35055104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="35056640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="35056640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="35055104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1226,6 +1384,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1524,7 +1712,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding stopping sharing with time
</commit_message>
<xml_diff>
--- a/data/excelsheets/Receptive sharing risk.xlsx
+++ b/data/excelsheets/Receptive sharing risk.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>http://www.ncbi.nlm.nih.gov/pubmed/23664499</t>
   </si>
@@ -100,6 +103,12 @@
   </si>
   <si>
     <t>Risk ratio of receptive injection</t>
+  </si>
+  <si>
+    <t>Per year rate</t>
+  </si>
+  <si>
+    <t>Per year probability</t>
   </si>
 </sst>
 </file>
@@ -584,9 +593,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -632,8 +642,36 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -737,11 +775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43546880"/>
-        <c:axId val="43560960"/>
+        <c:axId val="46903680"/>
+        <c:axId val="46905216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43546880"/>
+        <c:axId val="46903680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,12 +789,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43560960"/>
+        <c:crossAx val="46905216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43560960"/>
+        <c:axId val="46905216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43546880"/>
+        <c:crossAx val="46903680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1115,11 +1153,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54466432"/>
-        <c:axId val="54467968"/>
+        <c:axId val="47075328"/>
+        <c:axId val="47076864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54466432"/>
+        <c:axId val="47075328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1166,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54467968"/>
+        <c:crossAx val="47076864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1136,7 +1174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54467968"/>
+        <c:axId val="47076864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1185,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54466432"/>
+        <c:crossAx val="47075328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1273,11 +1311,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="35055104"/>
-        <c:axId val="35056640"/>
+        <c:axId val="47101056"/>
+        <c:axId val="47102592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35055104"/>
+        <c:axId val="47101056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35056640"/>
+        <c:crossAx val="47102592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1294,7 +1332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35056640"/>
+        <c:axId val="47102592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,7 +1343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35055104"/>
+        <c:crossAx val="47101056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1712,7 +1750,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1783,7 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1771,7 +1809,7 @@
         <f>D5</f>
         <v>0.1598360655737705</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <f>G9/G5</f>
         <v>0.59807040417209911</v>
       </c>
@@ -1819,6 +1857,13 @@
         <f t="shared" si="1"/>
         <v>0.12327718223583461</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1840,6 +1885,15 @@
       <c r="G8">
         <f t="shared" si="1"/>
         <v>0.12035010940919037</v>
+      </c>
+      <c r="I8" s="2">
+        <f>I5^(1/22)</f>
+        <v>0.97690510209022707</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2">
+        <f>1-I8</f>
+        <v>2.3094897909772927E-2</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>